<commit_message>
Se actualiza parte de la interfaz navbar y footer a demas se agregan las fotos definitivas y un video
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DenyingCarrot\Desktop\Experiencia1_Fuenzalida_002D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DenyingCarrot\Desktop\Experiencia1_Fuenzalida_002D\Experiencia1_Fuenzalida_002D\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13080" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="BitácoraExperiencia1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>Equipo</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>Desarrollo Pagina de Inicio</t>
+  </si>
+  <si>
+    <t>Desarrollo Pagina Quienes Somos</t>
+  </si>
+  <si>
+    <t>Desarrollo Pagina con Galeria de Fotos</t>
   </si>
 </sst>
 </file>
@@ -437,7 +443,7 @@
   <dimension ref="B2:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,6 +514,9 @@
       <c r="B9" s="2">
         <v>3</v>
       </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
       <c r="D9" t="s">
         <v>6</v>
       </c>
@@ -515,6 +524,9 @@
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Se finaliza la pagina de galeria y se añaden las tareas realizadas en la bitacora
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>Equipo</t>
   </si>
@@ -66,6 +66,21 @@
   </si>
   <si>
     <t>Desarrollo Pagina con Galeria de Fotos</t>
+  </si>
+  <si>
+    <t>Mejora en diseño de navbar</t>
+  </si>
+  <si>
+    <t>Mejora en diseño de footer</t>
+  </si>
+  <si>
+    <t>Implementacion de imágenes y videos</t>
+  </si>
+  <si>
+    <t>Recopilacion de informacion</t>
+  </si>
+  <si>
+    <t>Ingreso de informacion relevante</t>
   </si>
 </sst>
 </file>
@@ -442,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,6 +551,9 @@
       <c r="B11" s="2">
         <v>5</v>
       </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
       <c r="D11" t="s">
         <v>6</v>
       </c>
@@ -543,6 +561,9 @@
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
@@ -552,6 +573,9 @@
       <c r="B13" s="2">
         <v>7</v>
       </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
@@ -560,6 +584,9 @@
       <c r="B14" s="2">
         <v>8</v>
       </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
       <c r="D14" t="s">
         <v>6</v>
       </c>
@@ -567,6 +594,9 @@
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Se corrige la ortografia actualiza la bitacora y completa la pagina de inicio y quienes somos
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>Equipo</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Ingreso de informacion relevante</t>
+  </si>
+  <si>
+    <t>Se agregan ultimos detalles para embellecer</t>
   </si>
 </sst>
 </file>
@@ -455,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D17"/>
+  <dimension ref="B2:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,7 +471,7 @@
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,7 +479,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -484,7 +487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -492,7 +495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -503,7 +506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>1</v>
       </c>
@@ -514,7 +517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>2</v>
       </c>
@@ -525,7 +528,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>3</v>
       </c>
@@ -536,7 +539,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>4</v>
       </c>
@@ -547,7 +550,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>5</v>
       </c>
@@ -558,7 +561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>6</v>
       </c>
@@ -569,7 +572,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>7</v>
       </c>
@@ -580,7 +583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>8</v>
       </c>
@@ -591,7 +594,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>9</v>
       </c>
@@ -601,10 +604,14 @@
       <c r="D15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>

</xml_diff>